<commit_message>
Corrections subject et derivedFrom
Modifications demandées par PFI:
Restreindre Subject à référencer Patient et
DerivedFrom à référencer seulement Observation et QuestionnaireResponse 2b8ba26c2748f94dcc436575d2bb8b9175dcb6c8
</commit_message>
<xml_diff>
--- a/ig/TLSVObservation/StructureDefinition-TLSVObservation.xlsx
+++ b/ig/TLSVObservation/StructureDefinition-TLSVObservation.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-12-21T15:44:28+00:00</t>
+    <t>2024-01-09T11:57:44+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -705,7 +705,7 @@
     <t>Observation.subject</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Patient|Group|Device|Location)
+    <t xml:space="preserve">Reference(Patient)
 </t>
   </si>
   <si>
@@ -1354,7 +1354,7 @@
     <t>Observation.derivedFrom</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(DocumentReference|ImagingStudy|Media|QuestionnaireResponse|Observation|MolecularSequence)
+    <t xml:space="preserve">Reference(QuestionnaireResponse|Observation)
 </t>
   </si>
   <si>

</xml_diff>